<commit_message>
Fixed cell colouring on creation, but can't get a button to colour the cells based on a room.
</commit_message>
<xml_diff>
--- a/EmergusQuestivo/EmergusQuestivo.xlsx
+++ b/EmergusQuestivo/EmergusQuestivo.xlsx
@@ -340,11 +340,24 @@
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R6b67d0625c574c96"/>
   </wetp:taskpane>
+  <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Ra0d0b422935c4f16"/>
+  </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
 <we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{5e7df604-fe3a-4bb8-8c4d-261bf4a0b217}">
+  <we:reference id="ca39c199-bb49-427d-9a89-4fe415bb28e9" version="1.0.0.0" store="developer" storeType="Registry"/>
+  <we:alternateReferences/>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
+<file path=xl/webextensions/webextension2.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{8d317218-5798-44d0-be2b-64742536e0a8}">
   <we:reference id="ca39c199-bb49-427d-9a89-4fe415bb28e9" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
IT'S WORKING. IT'S WORKING!
</commit_message>
<xml_diff>
--- a/EmergusQuestivo/EmergusQuestivo.xlsx
+++ b/EmergusQuestivo/EmergusQuestivo.xlsx
@@ -343,6 +343,9 @@
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Ra0d0b422935c4f16"/>
   </wetp:taskpane>
+  <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rdc95b6144e7e40b2"/>
+  </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
@@ -358,6 +361,16 @@
 
 <file path=xl/webextensions/webextension2.xml><?xml version="1.0" encoding="utf-8"?>
 <we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{8d317218-5798-44d0-be2b-64742536e0a8}">
+  <we:reference id="ca39c199-bb49-427d-9a89-4fe415bb28e9" version="1.0.0.0" store="developer" storeType="Registry"/>
+  <we:alternateReferences/>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
+<file path=xl/webextensions/webextension3.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{03b62139-2721-437d-8fcb-c20b8ec6db8a}">
   <we:reference id="ca39c199-bb49-427d-9a89-4fe415bb28e9" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Got the set character code to work along with changing font color and size - KW
</commit_message>
<xml_diff>
--- a/EmergusQuestivo/EmergusQuestivo.xlsx
+++ b/EmergusQuestivo/EmergusQuestivo.xlsx
@@ -346,6 +346,9 @@
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rdc95b6144e7e40b2"/>
   </wetp:taskpane>
+  <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Re60413775a0545d5"/>
+  </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
@@ -371,6 +374,16 @@
 
 <file path=xl/webextensions/webextension3.xml><?xml version="1.0" encoding="utf-8"?>
 <we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{03b62139-2721-437d-8fcb-c20b8ec6db8a}">
+  <we:reference id="ca39c199-bb49-427d-9a89-4fe415bb28e9" version="1.0.0.0" store="developer" storeType="Registry"/>
+  <we:alternateReferences/>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
+<file path=xl/webextensions/webextension4.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{87ed4559-370e-49b3-bd08-165280b72485}">
   <we:reference id="ca39c199-bb49-427d-9a89-4fe415bb28e9" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Rooms and their contents
</commit_message>
<xml_diff>
--- a/EmergusQuestivo/EmergusQuestivo.xlsx
+++ b/EmergusQuestivo/EmergusQuestivo.xlsx
@@ -349,6 +349,9 @@
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Re60413775a0545d5"/>
   </wetp:taskpane>
+  <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rdc091ae3bb4e41f3"/>
+  </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
@@ -384,6 +387,16 @@
 
 <file path=xl/webextensions/webextension4.xml><?xml version="1.0" encoding="utf-8"?>
 <we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{87ed4559-370e-49b3-bd08-165280b72485}">
+  <we:reference id="ca39c199-bb49-427d-9a89-4fe415bb28e9" version="1.0.0.0" store="developer" storeType="Registry"/>
+  <we:alternateReferences/>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
+<file path=xl/webextensions/webextension5.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{848a9a60-8fac-46a9-b8c7-959901d368c2}">
   <we:reference id="ca39c199-bb49-427d-9a89-4fe415bb28e9" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Working on populating room items KW
</commit_message>
<xml_diff>
--- a/EmergusQuestivo/EmergusQuestivo.xlsx
+++ b/EmergusQuestivo/EmergusQuestivo.xlsx
@@ -352,6 +352,9 @@
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rdc091ae3bb4e41f3"/>
   </wetp:taskpane>
+  <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R66e263933a144ace"/>
+  </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
@@ -397,6 +400,16 @@
 
 <file path=xl/webextensions/webextension5.xml><?xml version="1.0" encoding="utf-8"?>
 <we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{848a9a60-8fac-46a9-b8c7-959901d368c2}">
+  <we:reference id="ca39c199-bb49-427d-9a89-4fe415bb28e9" version="1.0.0.0" store="developer" storeType="Registry"/>
+  <we:alternateReferences/>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
+<file path=xl/webextensions/webextension6.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{5f799f4a-ccff-4ead-bd5b-f58db9425777}">
   <we:reference id="ca39c199-bb49-427d-9a89-4fe415bb28e9" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>